<commit_message>
This is update but I can't remember what I updated, I'm sorry.
</commit_message>
<xml_diff>
--- a/data/Test_Results.xlsx
+++ b/data/Test_Results.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
   <si>
     <t>Lot</t>
   </si>
@@ -23,6 +29,24 @@
   </si>
   <si>
     <t>Yield</t>
+  </si>
+  <si>
+    <t>W118892</t>
+  </si>
+  <si>
+    <t>R114792-03</t>
+  </si>
+  <si>
+    <t>99.97%</t>
+  </si>
+  <si>
+    <t>GAL-LOT</t>
+  </si>
+  <si>
+    <t>GAL-LOT-02</t>
+  </si>
+  <si>
+    <t>GAL-LOT-03</t>
   </si>
 </sst>
 </file>
@@ -354,45 +378,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C1:E4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="3:5">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="3:5">
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
+    <row r="2" spans="1:5">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="3:5">
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
+    <row r="3" spans="1:5">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>35</v>
+    <row r="4" spans="1:5">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>